<commit_message>
225488 Add support for new token format
</commit_message>
<xml_diff>
--- a/tests/pricelist_files/PRC-1234-1234-1234.xlsx
+++ b/tests/pricelist_files/PRC-1234-1234-1234.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavellonkin/Documents/git/swo-marketplace-cli/tests/pricelist_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB8CC40-DEF0-4F4B-99E7-1F37F424ABB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E2FF86-D576-7149-9AEE-32A9CFF322B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,9 +1028,7 @@
       <c r="N5" s="9">
         <v>0.3</v>
       </c>
-      <c r="O5" s="9">
-        <v>15.55</v>
-      </c>
+      <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>

</xml_diff>